<commit_message>
Exel filters and formulae basics
</commit_message>
<xml_diff>
--- a/day1.xlsx
+++ b/day1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cadd Mentor\Student_Class_Code\Jazaul_Hasan_Data_Anylytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE833E5-653D-4EAC-ACE0-835275A54756}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A5EA3C-F8C9-41B5-9108-E00E263FFF5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_ [$₹-4009]\ * #,##0.00_ ;_ [$₹-4009]\ * \-#,##0.00_ ;_ [$₹-4009]\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ [$₹-4009]\ * #,##0.00_ ;_ [$₹-4009]\ * \-#,##0.00_ ;_ [$₹-4009]\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -181,18 +181,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -200,17 +200,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -510,7 +500,7 @@
   <dimension ref="D3:I11"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,13 +513,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
@@ -538,74 +528,74 @@
       <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="12"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>456.56700000000001</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>65476</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>45728</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>2.3333333333333335</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="12"/>
+      <c r="I4" s="11"/>
     </row>
     <row r="5" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>4356.4560000000001</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>436</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>46122</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>0.75</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>345.45670000000001</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>3465</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="10" t="s">
+      <c r="F6" s="8"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="11"/>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D8" s="7"/>
-      <c r="F8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="F9" s="5"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="F10" s="5"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="F11" s="5"/>
+      <c r="F11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -616,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8DF91A-7B26-42AB-8E80-D60A63636B14}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,12 +617,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -720,7 +710,7 @@
   <dimension ref="D5:O21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="D5" sqref="D5:O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1285,11 +1275,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="O6:O10">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Peter">
-      <formula>NOT(ISERROR(SEARCH("Peter",O6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1298,8 +1283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32C5421-1F96-4D1B-BB4C-77D749DBAFB2}">
   <dimension ref="D4:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>